<commit_message>
Population Mean Centers Calculated
</commit_message>
<xml_diff>
--- a/Lab2/Lab2_data/Lab2_data/Tables/MD 1900 1990 MSP.xlsx
+++ b/Lab2/Lab2_data/Lab2_data/Tables/MD 1900 1990 MSP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lostk\OneDrive\Desktop\Working Directory\Schule\Lab2\Lab2_data\Lab2_data\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6981C25-4C3C-4435-B1C9-7F30AB8CAF30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E2A48C-BEAB-472A-BED7-268DE6E7A6D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{63502ACE-C444-435B-9A56-513FF61751BD}"/>
   </bookViews>
@@ -45,8 +45,30 @@
 </connections>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="374">
   <si>
     <t>Column1</t>
   </si>
@@ -1093,13 +1115,88 @@
   </si>
   <si>
     <t>CENTROID_Y_RAD</t>
+  </si>
+  <si>
+    <t>LATITUDE1900</t>
+  </si>
+  <si>
+    <t>LONGITUDE1900</t>
+  </si>
+  <si>
+    <t>LATITUDE1910</t>
+  </si>
+  <si>
+    <t>LATITUDE1920</t>
+  </si>
+  <si>
+    <t>LATITUDE1930</t>
+  </si>
+  <si>
+    <t>LATITUDE1940</t>
+  </si>
+  <si>
+    <t>LATITUDE1950</t>
+  </si>
+  <si>
+    <t>LATITUDE1960</t>
+  </si>
+  <si>
+    <t>LATITUDE1970</t>
+  </si>
+  <si>
+    <t>LATITUDE1980</t>
+  </si>
+  <si>
+    <t>LATITUDE1990</t>
+  </si>
+  <si>
+    <t>LATITUDE2000</t>
+  </si>
+  <si>
+    <t>LATITUDE2008</t>
+  </si>
+  <si>
+    <t>LONGITUDE1910</t>
+  </si>
+  <si>
+    <t>LONGITUDE1920</t>
+  </si>
+  <si>
+    <t>LONGITUDE1930</t>
+  </si>
+  <si>
+    <t>LONGITUDE1940</t>
+  </si>
+  <si>
+    <t>LONGITUDE1950</t>
+  </si>
+  <si>
+    <t>LONGITUDE1960</t>
+  </si>
+  <si>
+    <t>LONGITUDE1970</t>
+  </si>
+  <si>
+    <t>LONGITUDE1980</t>
+  </si>
+  <si>
+    <t>LONGITUDE1990</t>
+  </si>
+  <si>
+    <t>LONGITUDE2000</t>
+  </si>
+  <si>
+    <t>LONGITUDE2008</t>
+  </si>
+  <si>
+    <t>Convert to Degrees</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1109,6 +1206,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1134,9 +1239,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1505,10 +1611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79AC8BBC-A864-4A82-99CA-A17289901047}">
-  <dimension ref="A1:R25"/>
+  <dimension ref="A1:AD25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1519,9 +1625,11 @@
     <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="17" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="30" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>331</v>
       </c>
@@ -1576,43 +1684,79 @@
       <c r="R1" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S1" t="s">
+        <v>349</v>
+      </c>
+      <c r="T1" t="s">
+        <v>351</v>
+      </c>
+      <c r="U1" t="s">
+        <v>352</v>
+      </c>
+      <c r="V1" t="s">
+        <v>353</v>
+      </c>
+      <c r="W1" t="s">
+        <v>354</v>
+      </c>
+      <c r="X1" t="s">
+        <v>355</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>356</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>357</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>358</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>359</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>360</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>31</v>
       </c>
       <c r="B2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" t="s">
-        <v>284</v>
-      </c>
-      <c r="D2" t="s">
-        <v>283</v>
-      </c>
-      <c r="E2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F2" t="s">
-        <v>184</v>
-      </c>
-      <c r="G2" t="s">
-        <v>183</v>
-      </c>
-      <c r="H2" t="s">
-        <v>182</v>
-      </c>
-      <c r="I2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" t="s">
-        <v>27</v>
+      <c r="C2" s="1">
+        <v>53694</v>
+      </c>
+      <c r="D2" s="1">
+        <v>62411</v>
+      </c>
+      <c r="E2" s="1">
+        <v>69938</v>
+      </c>
+      <c r="F2" s="1">
+        <v>79098</v>
+      </c>
+      <c r="G2" s="1">
+        <v>86973</v>
+      </c>
+      <c r="H2" s="1">
+        <v>89556</v>
+      </c>
+      <c r="I2" s="1">
+        <v>84169</v>
+      </c>
+      <c r="J2" s="1">
+        <v>84044</v>
+      </c>
+      <c r="K2" s="1">
+        <v>80548</v>
+      </c>
+      <c r="L2" s="1">
+        <v>74946</v>
       </c>
       <c r="M2">
         <v>74807</v>
@@ -1634,43 +1778,91 @@
         <f>P2*(PI()/180)</f>
         <v>0.68057690422712191</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S2">
+        <f>SUMPRODUCT(C2:C25,$R$2:$R$25)/SUM(C2:C25)</f>
+        <v>0.67508437063225324</v>
+      </c>
+      <c r="T2">
+        <f>SUMPRODUCT(D2:D25,$R$2:$R$25)/SUM(D2:D25)</f>
+        <v>0.67507816906053786</v>
+      </c>
+      <c r="U2">
+        <f>SUMPRODUCT(E2:E25,$R$2:$R$25)/SUM(E2:E25)</f>
+        <v>0.67396276024426982</v>
+      </c>
+      <c r="V2">
+        <f t="shared" ref="V2:AD2" si="0">SUMPRODUCT(F2:F25,$R$2:$R$25)/SUM(F2:F25)</f>
+        <v>0.67420786705705171</v>
+      </c>
+      <c r="W2">
+        <f t="shared" si="0"/>
+        <v>0.67468054343332173</v>
+      </c>
+      <c r="X2">
+        <f t="shared" si="0"/>
+        <v>0.67585383724192372</v>
+      </c>
+      <c r="Y2">
+        <f t="shared" si="0"/>
+        <v>0.67768468590280728</v>
+      </c>
+      <c r="Z2">
+        <f t="shared" si="0"/>
+        <v>0.67907858085750583</v>
+      </c>
+      <c r="AA2">
+        <f t="shared" si="0"/>
+        <v>0.67963948607421087</v>
+      </c>
+      <c r="AB2">
+        <f t="shared" si="0"/>
+        <v>0.68032395943816659</v>
+      </c>
+      <c r="AC2">
+        <f t="shared" si="0"/>
+        <v>0.680822613647312</v>
+      </c>
+      <c r="AD2">
+        <f t="shared" si="0"/>
+        <v>0.68098600791130792</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
       </c>
-      <c r="C3" t="s">
-        <v>286</v>
-      </c>
-      <c r="D3" t="s">
-        <v>285</v>
-      </c>
-      <c r="E3" t="s">
-        <v>189</v>
-      </c>
-      <c r="F3" t="s">
-        <v>188</v>
-      </c>
-      <c r="G3" t="s">
-        <v>187</v>
-      </c>
-      <c r="H3" t="s">
-        <v>186</v>
-      </c>
-      <c r="I3" t="s">
-        <v>36</v>
-      </c>
-      <c r="J3" t="s">
-        <v>35</v>
-      </c>
-      <c r="K3" t="s">
-        <v>34</v>
-      </c>
-      <c r="L3" t="s">
-        <v>33</v>
+      <c r="C3" s="1">
+        <v>39620</v>
+      </c>
+      <c r="D3" s="1">
+        <v>39553</v>
+      </c>
+      <c r="E3" s="1">
+        <v>43408</v>
+      </c>
+      <c r="F3" s="1">
+        <v>55167</v>
+      </c>
+      <c r="G3" s="1">
+        <v>68375</v>
+      </c>
+      <c r="H3" s="1">
+        <v>117392</v>
+      </c>
+      <c r="I3" s="1">
+        <v>206634</v>
+      </c>
+      <c r="J3" s="1">
+        <v>297539</v>
+      </c>
+      <c r="K3" s="1">
+        <v>370775</v>
+      </c>
+      <c r="L3" s="1">
+        <v>427239</v>
       </c>
       <c r="M3">
         <v>491331</v>
@@ -1685,50 +1877,50 @@
         <v>38.079283277979528</v>
       </c>
       <c r="Q3">
-        <f t="shared" ref="Q3:Q25" si="0">O3*(PI()/180)</f>
+        <f t="shared" ref="Q3:Q25" si="1">O3*(PI()/180)</f>
         <v>-1.3238837673102655</v>
       </c>
       <c r="R3">
-        <f t="shared" ref="R3:R25" si="1">P3*(PI()/180)</f>
+        <f t="shared" ref="R3:R25" si="2">P3*(PI()/180)</f>
         <v>0.66460887000036195</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>43</v>
       </c>
       <c r="B4" t="s">
         <v>38</v>
       </c>
-      <c r="C4" t="s">
-        <v>288</v>
-      </c>
-      <c r="D4" t="s">
-        <v>287</v>
-      </c>
-      <c r="E4" t="s">
-        <v>193</v>
-      </c>
-      <c r="F4" t="s">
-        <v>192</v>
-      </c>
-      <c r="G4" t="s">
-        <v>191</v>
-      </c>
-      <c r="H4" t="s">
-        <v>190</v>
-      </c>
-      <c r="I4" t="s">
-        <v>42</v>
-      </c>
-      <c r="J4" t="s">
-        <v>41</v>
-      </c>
-      <c r="K4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L4" t="s">
-        <v>39</v>
+      <c r="C4" s="1">
+        <v>90755</v>
+      </c>
+      <c r="D4" s="1">
+        <v>122349</v>
+      </c>
+      <c r="E4" s="1">
+        <v>74817</v>
+      </c>
+      <c r="F4" s="1">
+        <v>124565</v>
+      </c>
+      <c r="G4" s="1">
+        <v>155825</v>
+      </c>
+      <c r="H4" s="1">
+        <v>270273</v>
+      </c>
+      <c r="I4" s="1">
+        <v>492428</v>
+      </c>
+      <c r="J4" s="1">
+        <v>621077</v>
+      </c>
+      <c r="K4" s="1">
+        <v>655615</v>
+      </c>
+      <c r="L4" s="1">
+        <v>692134</v>
       </c>
       <c r="M4">
         <v>755992</v>
@@ -1743,50 +1935,86 @@
         <v>39.136347563743684</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.3474685302052172</v>
       </c>
       <c r="R4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.68305812219218864</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S4" t="s">
+        <v>350</v>
+      </c>
+      <c r="T4" t="s">
+        <v>362</v>
+      </c>
+      <c r="U4" t="s">
+        <v>363</v>
+      </c>
+      <c r="V4" t="s">
+        <v>364</v>
+      </c>
+      <c r="W4" t="s">
+        <v>365</v>
+      </c>
+      <c r="X4" t="s">
+        <v>366</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>367</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>368</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>369</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>370</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>371</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>49</v>
       </c>
       <c r="B5" t="s">
         <v>44</v>
       </c>
-      <c r="C5" t="s">
-        <v>290</v>
-      </c>
-      <c r="D5" t="s">
-        <v>289</v>
-      </c>
-      <c r="E5" t="s">
-        <v>197</v>
-      </c>
-      <c r="F5" t="s">
-        <v>196</v>
-      </c>
-      <c r="G5" t="s">
-        <v>195</v>
-      </c>
-      <c r="H5" t="s">
-        <v>194</v>
-      </c>
-      <c r="I5" t="s">
-        <v>48</v>
-      </c>
-      <c r="J5" t="s">
-        <v>47</v>
-      </c>
-      <c r="K5" t="s">
-        <v>46</v>
-      </c>
-      <c r="L5" t="s">
-        <v>45</v>
+      <c r="C5" s="1">
+        <v>10223</v>
+      </c>
+      <c r="D5" s="1">
+        <v>10325</v>
+      </c>
+      <c r="E5" s="1">
+        <v>9744</v>
+      </c>
+      <c r="F5" s="1">
+        <v>9528</v>
+      </c>
+      <c r="G5" s="1">
+        <v>10484</v>
+      </c>
+      <c r="H5" s="1">
+        <v>12100</v>
+      </c>
+      <c r="I5" s="1">
+        <v>15826</v>
+      </c>
+      <c r="J5" s="1">
+        <v>20682</v>
+      </c>
+      <c r="K5" s="1">
+        <v>34638</v>
+      </c>
+      <c r="L5" s="1">
+        <v>51372</v>
       </c>
       <c r="M5">
         <v>75164</v>
@@ -1801,50 +2029,98 @@
         <v>38.212856521135649</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.3148226757412731</v>
       </c>
       <c r="R5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.66694016288600322</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S5" cm="1">
+        <f t="array" ref="S5">(SUMPRODUCT(C2:C25,$Q$2:$Q$25,COS($R$2:$R$25))/SUMPRODUCT(C2:C25,COS($R$2:$R$25)))</f>
+        <v>-1.338157975612204</v>
+      </c>
+      <c r="T5" cm="1">
+        <f t="array" ref="T5">(SUMPRODUCT(D2:D25,$Q$2:$Q$25,COS($R$2:$R$25))/SUMPRODUCT(D2:D25,COS($R$2:$R$25)))</f>
+        <v>-1.338227051939781</v>
+      </c>
+      <c r="U5" cm="1">
+        <f t="array" ref="U5">(SUMPRODUCT(E2:E25,$Q$2:$Q$25,COS($R$2:$R$25))/SUMPRODUCT(E2:E25,COS($R$2:$R$25)))</f>
+        <v>-1.3376672846228974</v>
+      </c>
+      <c r="V5" cm="1">
+        <f t="array" ref="V5">(SUMPRODUCT(F2:F25,$Q$2:$Q$25,COS($R$2:$R$25))/SUMPRODUCT(F2:F25,COS($R$2:$R$25)))</f>
+        <v>-1.3382273018440491</v>
+      </c>
+      <c r="W5" cm="1">
+        <f t="array" ref="W5">(SUMPRODUCT(G2:G25,$Q$2:$Q$25,COS($R$2:$R$25))/SUMPRODUCT(G2:G25,COS($R$2:$R$25)))</f>
+        <v>-1.3391436568138912</v>
+      </c>
+      <c r="X5" cm="1">
+        <f t="array" ref="X5">(SUMPRODUCT(H2:H25,$Q$2:$Q$25,COS($R$2:$R$25))/SUMPRODUCT(H2:H25,COS($R$2:$R$25)))</f>
+        <v>-1.3409357968179714</v>
+      </c>
+      <c r="Y5" cm="1">
+        <f t="array" ref="Y5">(SUMPRODUCT(I2:I25,$Q$2:$Q$25,COS($R$2:$R$25))/SUMPRODUCT(I2:I25,COS($R$2:$R$25)))</f>
+        <v>-1.3435014765115203</v>
+      </c>
+      <c r="Z5" cm="1">
+        <f t="array" ref="Z5">(SUMPRODUCT(J2:J25,$Q$2:$Q$25,COS($R$2:$R$25))/SUMPRODUCT(J2:J25,COS($R$2:$R$25)))</f>
+        <v>-1.3450786282193454</v>
+      </c>
+      <c r="AA5" cm="1">
+        <f t="array" ref="AA5">(SUMPRODUCT(K2:K25,$Q$2:$Q$25,COS($R$2:$R$25))/SUMPRODUCT(K2:K25,COS($R$2:$R$25)))</f>
+        <v>-1.3451773039058976</v>
+      </c>
+      <c r="AB5" cm="1">
+        <f t="array" ref="AB5">(SUMPRODUCT(L2:L25,$Q$2:$Q$25,COS($R$2:$R$25))/SUMPRODUCT(L2:L25,COS($R$2:$R$25)))</f>
+        <v>-1.3460783809206547</v>
+      </c>
+      <c r="AC5" cm="1">
+        <f t="array" ref="AC5">(SUMPRODUCT(M2:M25,$Q$2:$Q$25,COS($R$2:$R$25))/SUMPRODUCT(M2:M25,COS($R$2:$R$25)))</f>
+        <v>-1.3464022634621224</v>
+      </c>
+      <c r="AD5" cm="1">
+        <f t="array" ref="AD5">(SUMPRODUCT(N2:N25,$Q$2:$Q$25,COS($R$2:$R$25))/SUMPRODUCT(N2:N25,COS($R$2:$R$25)))</f>
+        <v>-1.3465677670525562</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>55</v>
       </c>
       <c r="B6" t="s">
         <v>50</v>
       </c>
-      <c r="C6" t="s">
-        <v>292</v>
-      </c>
-      <c r="D6" t="s">
-        <v>291</v>
-      </c>
-      <c r="E6" t="s">
-        <v>201</v>
-      </c>
-      <c r="F6" t="s">
-        <v>200</v>
-      </c>
-      <c r="G6" t="s">
-        <v>199</v>
-      </c>
-      <c r="H6" t="s">
-        <v>198</v>
-      </c>
-      <c r="I6" t="s">
-        <v>54</v>
-      </c>
-      <c r="J6" t="s">
-        <v>53</v>
-      </c>
-      <c r="K6" t="s">
-        <v>52</v>
-      </c>
-      <c r="L6" t="s">
-        <v>51</v>
+      <c r="C6" s="1">
+        <v>16248</v>
+      </c>
+      <c r="D6" s="1">
+        <v>19216</v>
+      </c>
+      <c r="E6" s="1">
+        <v>18652</v>
+      </c>
+      <c r="F6" s="1">
+        <v>17387</v>
+      </c>
+      <c r="G6" s="1">
+        <v>17549</v>
+      </c>
+      <c r="H6" s="1">
+        <v>18234</v>
+      </c>
+      <c r="I6" s="1">
+        <v>19462</v>
+      </c>
+      <c r="J6" s="1">
+        <v>19781</v>
+      </c>
+      <c r="K6" s="1">
+        <v>23143</v>
+      </c>
+      <c r="L6" s="1">
+        <v>27035</v>
       </c>
       <c r="M6">
         <v>29825</v>
@@ -1859,50 +2135,50 @@
         <v>39.537489242007616</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.3316687294487968</v>
       </c>
       <c r="R6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.69005936524486999</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>61</v>
       </c>
       <c r="B7" t="s">
         <v>56</v>
       </c>
-      <c r="C7" t="s">
-        <v>294</v>
-      </c>
-      <c r="D7" t="s">
-        <v>293</v>
-      </c>
-      <c r="E7" t="s">
-        <v>205</v>
-      </c>
-      <c r="F7" t="s">
-        <v>204</v>
-      </c>
-      <c r="G7" t="s">
-        <v>203</v>
-      </c>
-      <c r="H7" t="s">
-        <v>202</v>
-      </c>
-      <c r="I7" t="s">
-        <v>60</v>
-      </c>
-      <c r="J7" t="s">
-        <v>59</v>
-      </c>
-      <c r="K7" t="s">
-        <v>58</v>
-      </c>
-      <c r="L7" t="s">
-        <v>57</v>
+      <c r="C7" s="1">
+        <v>33860</v>
+      </c>
+      <c r="D7" s="1">
+        <v>33934</v>
+      </c>
+      <c r="E7" s="1">
+        <v>34245</v>
+      </c>
+      <c r="F7" s="1">
+        <v>35978</v>
+      </c>
+      <c r="G7" s="1">
+        <v>39054</v>
+      </c>
+      <c r="H7" s="1">
+        <v>44907</v>
+      </c>
+      <c r="I7" s="1">
+        <v>52785</v>
+      </c>
+      <c r="J7" s="1">
+        <v>69006</v>
+      </c>
+      <c r="K7" s="1">
+        <v>96356</v>
+      </c>
+      <c r="L7" s="1">
+        <v>123372</v>
       </c>
       <c r="M7">
         <v>151577</v>
@@ -1917,50 +2193,53 @@
         <v>39.603703827125052</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.3581123972543845</v>
       </c>
       <c r="R7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.69121502776801136</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S7" s="2" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>67</v>
       </c>
       <c r="B8" t="s">
         <v>62</v>
       </c>
-      <c r="C8" t="s">
-        <v>296</v>
-      </c>
-      <c r="D8" t="s">
-        <v>295</v>
-      </c>
-      <c r="E8" t="s">
-        <v>209</v>
-      </c>
-      <c r="F8" t="s">
-        <v>208</v>
-      </c>
-      <c r="G8" t="s">
-        <v>207</v>
-      </c>
-      <c r="H8" t="s">
-        <v>206</v>
-      </c>
-      <c r="I8" t="s">
-        <v>66</v>
-      </c>
-      <c r="J8" t="s">
-        <v>65</v>
-      </c>
-      <c r="K8" t="s">
-        <v>64</v>
-      </c>
-      <c r="L8" t="s">
-        <v>63</v>
+      <c r="C8" s="1">
+        <v>24662</v>
+      </c>
+      <c r="D8" s="1">
+        <v>23759</v>
+      </c>
+      <c r="E8" s="1">
+        <v>23612</v>
+      </c>
+      <c r="F8" s="1">
+        <v>25827</v>
+      </c>
+      <c r="G8" s="1">
+        <v>26407</v>
+      </c>
+      <c r="H8" s="1">
+        <v>33356</v>
+      </c>
+      <c r="I8" s="1">
+        <v>48408</v>
+      </c>
+      <c r="J8" s="1">
+        <v>53291</v>
+      </c>
+      <c r="K8" s="1">
+        <v>60430</v>
+      </c>
+      <c r="L8" s="1">
+        <v>71347</v>
       </c>
       <c r="M8">
         <v>86465</v>
@@ -1975,50 +2254,86 @@
         <v>39.440627364184543</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.3371506094412884</v>
       </c>
       <c r="R8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.6883688065571929</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S8" t="s">
+        <v>349</v>
+      </c>
+      <c r="T8" t="s">
+        <v>351</v>
+      </c>
+      <c r="U8" t="s">
+        <v>352</v>
+      </c>
+      <c r="V8" t="s">
+        <v>353</v>
+      </c>
+      <c r="W8" t="s">
+        <v>354</v>
+      </c>
+      <c r="X8" t="s">
+        <v>355</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>356</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>357</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>358</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>359</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>360</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>73</v>
       </c>
       <c r="B9" t="s">
         <v>68</v>
       </c>
-      <c r="C9" t="s">
-        <v>298</v>
-      </c>
-      <c r="D9" t="s">
-        <v>297</v>
-      </c>
-      <c r="E9" t="s">
-        <v>213</v>
-      </c>
-      <c r="F9" t="s">
-        <v>212</v>
-      </c>
-      <c r="G9" t="s">
-        <v>211</v>
-      </c>
-      <c r="H9" t="s">
-        <v>210</v>
-      </c>
-      <c r="I9" t="s">
-        <v>72</v>
-      </c>
-      <c r="J9" t="s">
-        <v>71</v>
-      </c>
-      <c r="K9" t="s">
-        <v>70</v>
-      </c>
-      <c r="L9" t="s">
-        <v>69</v>
+      <c r="C9" s="1">
+        <v>17662</v>
+      </c>
+      <c r="D9" s="1">
+        <v>16386</v>
+      </c>
+      <c r="E9" s="1">
+        <v>17705</v>
+      </c>
+      <c r="F9" s="1">
+        <v>16166</v>
+      </c>
+      <c r="G9" s="1">
+        <v>17612</v>
+      </c>
+      <c r="H9" s="1">
+        <v>23415</v>
+      </c>
+      <c r="I9" s="1">
+        <v>32572</v>
+      </c>
+      <c r="J9" s="1">
+        <v>47678</v>
+      </c>
+      <c r="K9" s="1">
+        <v>72751</v>
+      </c>
+      <c r="L9" s="1">
+        <v>101154</v>
       </c>
       <c r="M9">
         <v>121204</v>
@@ -2033,50 +2348,98 @@
         <v>39.301019915908562</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.3371093100266009</v>
       </c>
       <c r="R9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.68593219692446938</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S9">
+        <f>S2*(180/PI())</f>
+        <v>38.679485252473526</v>
+      </c>
+      <c r="T9">
+        <f t="shared" ref="T9:AD9" si="3">T2*(180/PI())</f>
+        <v>38.679129928587891</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="3"/>
+        <v>38.615221710984045</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="3"/>
+        <v>38.629265296886352</v>
+      </c>
+      <c r="W9">
+        <f t="shared" si="3"/>
+        <v>38.656347658322161</v>
+      </c>
+      <c r="X9">
+        <f t="shared" si="3"/>
+        <v>38.723572441683885</v>
+      </c>
+      <c r="Y9">
+        <f t="shared" si="3"/>
+        <v>38.828472342879692</v>
+      </c>
+      <c r="Z9">
+        <f t="shared" si="3"/>
+        <v>38.908336640868498</v>
+      </c>
+      <c r="AA9">
+        <f t="shared" si="3"/>
+        <v>38.940474142492569</v>
+      </c>
+      <c r="AB9">
+        <f t="shared" si="3"/>
+        <v>38.979691577436355</v>
+      </c>
+      <c r="AC9">
+        <f t="shared" si="3"/>
+        <v>39.008262359056822</v>
+      </c>
+      <c r="AD9">
+        <f t="shared" si="3"/>
+        <v>39.017624160780436</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>79</v>
       </c>
       <c r="B10" t="s">
         <v>74</v>
       </c>
-      <c r="C10" t="s">
-        <v>300</v>
-      </c>
-      <c r="D10" t="s">
-        <v>299</v>
-      </c>
-      <c r="E10" t="s">
-        <v>217</v>
-      </c>
-      <c r="F10" t="s">
-        <v>216</v>
-      </c>
-      <c r="G10" t="s">
-        <v>215</v>
-      </c>
-      <c r="H10" t="s">
-        <v>214</v>
-      </c>
-      <c r="I10" t="s">
-        <v>78</v>
-      </c>
-      <c r="J10" t="s">
-        <v>77</v>
-      </c>
-      <c r="K10" t="s">
-        <v>76</v>
-      </c>
-      <c r="L10" t="s">
-        <v>75</v>
+      <c r="C10" s="1">
+        <v>27962</v>
+      </c>
+      <c r="D10" s="1">
+        <v>28669</v>
+      </c>
+      <c r="E10" s="1">
+        <v>27895</v>
+      </c>
+      <c r="F10" s="1">
+        <v>26813</v>
+      </c>
+      <c r="G10" s="1">
+        <v>28006</v>
+      </c>
+      <c r="H10" s="1">
+        <v>27815</v>
+      </c>
+      <c r="I10" s="1">
+        <v>29666</v>
+      </c>
+      <c r="J10" s="1">
+        <v>29405</v>
+      </c>
+      <c r="K10" s="1">
+        <v>30623</v>
+      </c>
+      <c r="L10" s="1">
+        <v>30236</v>
       </c>
       <c r="M10">
         <v>30586</v>
@@ -2091,50 +2454,50 @@
         <v>39.236075146731061</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.3280632869734617</v>
       </c>
       <c r="R10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.68479869687037431</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>85</v>
       </c>
       <c r="B11" t="s">
         <v>80</v>
       </c>
-      <c r="C11" t="s">
-        <v>302</v>
-      </c>
-      <c r="D11" t="s">
-        <v>301</v>
-      </c>
-      <c r="E11" t="s">
-        <v>221</v>
-      </c>
-      <c r="F11" t="s">
-        <v>220</v>
-      </c>
-      <c r="G11" t="s">
-        <v>219</v>
-      </c>
-      <c r="H11" t="s">
-        <v>218</v>
-      </c>
-      <c r="I11" t="s">
-        <v>84</v>
-      </c>
-      <c r="J11" t="s">
-        <v>83</v>
-      </c>
-      <c r="K11" t="s">
-        <v>82</v>
-      </c>
-      <c r="L11" t="s">
-        <v>81</v>
+      <c r="C11" s="1">
+        <v>51920</v>
+      </c>
+      <c r="D11" s="1">
+        <v>52673</v>
+      </c>
+      <c r="E11" s="1">
+        <v>52541</v>
+      </c>
+      <c r="F11" s="1">
+        <v>54440</v>
+      </c>
+      <c r="G11" s="1">
+        <v>57312</v>
+      </c>
+      <c r="H11" s="1">
+        <v>62287</v>
+      </c>
+      <c r="I11" s="1">
+        <v>71930</v>
+      </c>
+      <c r="J11" s="1">
+        <v>84927</v>
+      </c>
+      <c r="K11" s="1">
+        <v>114792</v>
+      </c>
+      <c r="L11" s="1">
+        <v>150208</v>
       </c>
       <c r="M11">
         <v>196501</v>
@@ -2149,50 +2512,86 @@
         <v>38.53431875697126</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.3356990021449873</v>
       </c>
       <c r="R11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.67255073732215709</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S11" t="s">
+        <v>350</v>
+      </c>
+      <c r="T11" t="s">
+        <v>362</v>
+      </c>
+      <c r="U11" t="s">
+        <v>363</v>
+      </c>
+      <c r="V11" t="s">
+        <v>364</v>
+      </c>
+      <c r="W11" t="s">
+        <v>365</v>
+      </c>
+      <c r="X11" t="s">
+        <v>366</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>367</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>368</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>369</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>370</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>371</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>91</v>
       </c>
       <c r="B12" t="s">
         <v>86</v>
       </c>
-      <c r="C12" t="s">
-        <v>304</v>
-      </c>
-      <c r="D12" t="s">
-        <v>303</v>
-      </c>
-      <c r="E12" t="s">
-        <v>225</v>
-      </c>
-      <c r="F12" t="s">
-        <v>224</v>
-      </c>
-      <c r="G12" t="s">
-        <v>223</v>
-      </c>
-      <c r="H12" t="s">
-        <v>222</v>
-      </c>
-      <c r="I12" t="s">
-        <v>90</v>
-      </c>
-      <c r="J12" t="s">
-        <v>89</v>
-      </c>
-      <c r="K12" t="s">
-        <v>88</v>
-      </c>
-      <c r="L12" t="s">
-        <v>87</v>
+      <c r="C12" s="1">
+        <v>17701</v>
+      </c>
+      <c r="D12" s="1">
+        <v>20105</v>
+      </c>
+      <c r="E12" s="1">
+        <v>19678</v>
+      </c>
+      <c r="F12" s="1">
+        <v>19908</v>
+      </c>
+      <c r="G12" s="1">
+        <v>21981</v>
+      </c>
+      <c r="H12" s="1">
+        <v>21259</v>
+      </c>
+      <c r="I12" s="1">
+        <v>20420</v>
+      </c>
+      <c r="J12" s="1">
+        <v>21476</v>
+      </c>
+      <c r="K12" s="1">
+        <v>26498</v>
+      </c>
+      <c r="L12" s="1">
+        <v>28138</v>
       </c>
       <c r="M12">
         <v>29824</v>
@@ -2207,50 +2606,98 @@
         <v>38.871729233622212</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.3235119809013134</v>
       </c>
       <c r="R12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.67843966107043963</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S12">
+        <f>S5*(180/PI())</f>
+        <v>-76.670804324349433</v>
+      </c>
+      <c r="T12">
+        <f t="shared" ref="T12:AD12" si="4">T5*(180/PI())</f>
+        <v>-76.674762106383852</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="4"/>
+        <v>-76.642689801617067</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="4"/>
+        <v>-76.674776424843699</v>
+      </c>
+      <c r="W12">
+        <f t="shared" si="4"/>
+        <v>-76.727279697151502</v>
+      </c>
+      <c r="X12">
+        <f t="shared" si="4"/>
+        <v>-76.82996175568185</v>
+      </c>
+      <c r="Y12">
+        <f t="shared" si="4"/>
+        <v>-76.976964373704618</v>
+      </c>
+      <c r="Z12">
+        <f t="shared" si="4"/>
+        <v>-77.06732851021485</v>
+      </c>
+      <c r="AA12">
+        <f t="shared" si="4"/>
+        <v>-77.072982210594844</v>
+      </c>
+      <c r="AB12">
+        <f t="shared" si="4"/>
+        <v>-77.124610120556667</v>
+      </c>
+      <c r="AC12">
+        <f t="shared" si="4"/>
+        <v>-77.143167223240738</v>
+      </c>
+      <c r="AD12">
+        <f t="shared" si="4"/>
+        <v>-77.152649880466853</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>97</v>
       </c>
       <c r="B13" t="s">
         <v>92</v>
       </c>
-      <c r="C13" t="s">
-        <v>306</v>
-      </c>
-      <c r="D13" t="s">
-        <v>305</v>
-      </c>
-      <c r="E13" t="s">
-        <v>229</v>
-      </c>
-      <c r="F13" t="s">
-        <v>228</v>
-      </c>
-      <c r="G13" t="s">
-        <v>227</v>
-      </c>
-      <c r="H13" t="s">
-        <v>226</v>
-      </c>
-      <c r="I13" t="s">
-        <v>96</v>
-      </c>
-      <c r="J13" t="s">
-        <v>95</v>
-      </c>
-      <c r="K13" t="s">
-        <v>94</v>
-      </c>
-      <c r="L13" t="s">
-        <v>93</v>
+      <c r="C13" s="1">
+        <v>28269</v>
+      </c>
+      <c r="D13" s="1">
+        <v>27965</v>
+      </c>
+      <c r="E13" s="1">
+        <v>29291</v>
+      </c>
+      <c r="F13" s="1">
+        <v>31603</v>
+      </c>
+      <c r="G13" s="1">
+        <v>35060</v>
+      </c>
+      <c r="H13" s="1">
+        <v>51782</v>
+      </c>
+      <c r="I13" s="1">
+        <v>76722</v>
+      </c>
+      <c r="J13" s="1">
+        <v>115378</v>
+      </c>
+      <c r="K13" s="1">
+        <v>145930</v>
+      </c>
+      <c r="L13" s="1">
+        <v>182132</v>
       </c>
       <c r="M13">
         <v>219464</v>
@@ -2265,50 +2712,50 @@
         <v>39.621166998303373</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.3734580460885457</v>
       </c>
       <c r="R13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.69151981760291237</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>103</v>
       </c>
       <c r="B14" t="s">
         <v>98</v>
       </c>
-      <c r="C14" t="s">
-        <v>308</v>
-      </c>
-      <c r="D14" t="s">
-        <v>307</v>
-      </c>
-      <c r="E14" t="s">
-        <v>48</v>
-      </c>
-      <c r="F14" t="s">
-        <v>232</v>
-      </c>
-      <c r="G14" t="s">
-        <v>231</v>
-      </c>
-      <c r="H14" t="s">
-        <v>230</v>
-      </c>
-      <c r="I14" t="s">
-        <v>102</v>
-      </c>
-      <c r="J14" t="s">
-        <v>101</v>
-      </c>
-      <c r="K14" t="s">
-        <v>100</v>
-      </c>
-      <c r="L14" t="s">
-        <v>99</v>
+      <c r="C14" s="1">
+        <v>16715</v>
+      </c>
+      <c r="D14" s="1">
+        <v>16106</v>
+      </c>
+      <c r="E14" s="1">
+        <v>15826</v>
+      </c>
+      <c r="F14" s="1">
+        <v>16169</v>
+      </c>
+      <c r="G14" s="1">
+        <v>17175</v>
+      </c>
+      <c r="H14" s="1">
+        <v>23119</v>
+      </c>
+      <c r="I14" s="1">
+        <v>36152</v>
+      </c>
+      <c r="J14" s="1">
+        <v>61911</v>
+      </c>
+      <c r="K14" s="1">
+        <v>118572</v>
+      </c>
+      <c r="L14" s="1">
+        <v>187328</v>
       </c>
       <c r="M14">
         <v>249520</v>
@@ -2323,50 +2770,50 @@
         <v>39.562467543071023</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.3255442934609136</v>
       </c>
       <c r="R14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.69049531883998083</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>109</v>
       </c>
       <c r="B15" t="s">
         <v>104</v>
       </c>
-      <c r="C15" t="s">
-        <v>310</v>
-      </c>
-      <c r="D15" t="s">
-        <v>309</v>
-      </c>
-      <c r="E15" t="s">
-        <v>236</v>
-      </c>
-      <c r="F15" t="s">
-        <v>235</v>
-      </c>
-      <c r="G15" t="s">
-        <v>234</v>
-      </c>
-      <c r="H15" t="s">
-        <v>233</v>
-      </c>
-      <c r="I15" t="s">
-        <v>108</v>
-      </c>
-      <c r="J15" t="s">
-        <v>107</v>
-      </c>
-      <c r="K15" t="s">
-        <v>106</v>
-      </c>
-      <c r="L15" t="s">
-        <v>105</v>
+      <c r="C15" s="1">
+        <v>18786</v>
+      </c>
+      <c r="D15" s="1">
+        <v>16957</v>
+      </c>
+      <c r="E15" s="1">
+        <v>15026</v>
+      </c>
+      <c r="F15" s="1">
+        <v>14242</v>
+      </c>
+      <c r="G15" s="1">
+        <v>13465</v>
+      </c>
+      <c r="H15" s="1">
+        <v>13677</v>
+      </c>
+      <c r="I15" s="1">
+        <v>15481</v>
+      </c>
+      <c r="J15" s="1">
+        <v>16146</v>
+      </c>
+      <c r="K15" s="1">
+        <v>16695</v>
+      </c>
+      <c r="L15" s="1">
+        <v>17842</v>
       </c>
       <c r="M15">
         <v>19267</v>
@@ -2381,50 +2828,50 @@
         <v>39.562872299142278</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.3442988188419713</v>
       </c>
       <c r="R15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.69050238316609169</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>115</v>
       </c>
       <c r="B16" t="s">
         <v>110</v>
       </c>
-      <c r="C16" t="s">
-        <v>312</v>
-      </c>
-      <c r="D16" t="s">
-        <v>311</v>
-      </c>
-      <c r="E16" t="s">
-        <v>240</v>
-      </c>
-      <c r="F16" t="s">
-        <v>239</v>
-      </c>
-      <c r="G16" t="s">
-        <v>238</v>
-      </c>
-      <c r="H16" t="s">
-        <v>237</v>
-      </c>
-      <c r="I16" t="s">
-        <v>114</v>
-      </c>
-      <c r="J16" t="s">
-        <v>113</v>
-      </c>
-      <c r="K16" t="s">
-        <v>112</v>
-      </c>
-      <c r="L16" t="s">
-        <v>111</v>
+      <c r="C16" s="1">
+        <v>30451</v>
+      </c>
+      <c r="D16" s="1">
+        <v>32089</v>
+      </c>
+      <c r="E16" s="1">
+        <v>34921</v>
+      </c>
+      <c r="F16" s="1">
+        <v>49206</v>
+      </c>
+      <c r="G16" s="1">
+        <v>83912</v>
+      </c>
+      <c r="H16" s="1">
+        <v>164401</v>
+      </c>
+      <c r="I16" s="1">
+        <v>340928</v>
+      </c>
+      <c r="J16" s="1">
+        <v>522809</v>
+      </c>
+      <c r="K16" s="1">
+        <v>579053</v>
+      </c>
+      <c r="L16" s="1">
+        <v>757027</v>
       </c>
       <c r="M16">
         <v>877495</v>
@@ -2439,11 +2886,11 @@
         <v>39.52987502107041</v>
       </c>
       <c r="Q16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.3835235463725262</v>
       </c>
       <c r="R16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.68992647201954149</v>
       </c>
     </row>
@@ -2454,35 +2901,35 @@
       <c r="B17" t="s">
         <v>116</v>
       </c>
-      <c r="C17" t="s">
-        <v>314</v>
-      </c>
-      <c r="D17" t="s">
-        <v>313</v>
-      </c>
-      <c r="E17" t="s">
-        <v>244</v>
-      </c>
-      <c r="F17" t="s">
-        <v>243</v>
-      </c>
-      <c r="G17" t="s">
-        <v>242</v>
-      </c>
-      <c r="H17" t="s">
-        <v>241</v>
-      </c>
-      <c r="I17" t="s">
-        <v>120</v>
-      </c>
-      <c r="J17" t="s">
-        <v>119</v>
-      </c>
-      <c r="K17" t="s">
-        <v>118</v>
-      </c>
-      <c r="L17" t="s">
-        <v>117</v>
+      <c r="C17" s="1">
+        <v>29898</v>
+      </c>
+      <c r="D17" s="1">
+        <v>36147</v>
+      </c>
+      <c r="E17" s="1">
+        <v>43347</v>
+      </c>
+      <c r="F17" s="1">
+        <v>60095</v>
+      </c>
+      <c r="G17" s="1">
+        <v>89490</v>
+      </c>
+      <c r="H17" s="1">
+        <v>194182</v>
+      </c>
+      <c r="I17" s="1">
+        <v>357395</v>
+      </c>
+      <c r="J17" s="1">
+        <v>660567</v>
+      </c>
+      <c r="K17" s="1">
+        <v>665071</v>
+      </c>
+      <c r="L17" s="1">
+        <v>729268</v>
       </c>
       <c r="M17">
         <v>803207</v>
@@ -2497,11 +2944,11 @@
         <v>39.250701442882573</v>
       </c>
       <c r="Q17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.3427034183324142</v>
       </c>
       <c r="R17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.68505397389558997</v>
       </c>
     </row>
@@ -2512,35 +2959,35 @@
       <c r="B18" t="s">
         <v>122</v>
       </c>
-      <c r="C18" t="s">
-        <v>316</v>
-      </c>
-      <c r="D18" t="s">
-        <v>315</v>
-      </c>
-      <c r="E18" t="s">
-        <v>248</v>
-      </c>
-      <c r="F18" t="s">
-        <v>247</v>
-      </c>
-      <c r="G18" t="s">
-        <v>246</v>
-      </c>
-      <c r="H18" t="s">
-        <v>245</v>
-      </c>
-      <c r="I18" t="s">
-        <v>126</v>
-      </c>
-      <c r="J18" t="s">
-        <v>125</v>
-      </c>
-      <c r="K18" t="s">
-        <v>124</v>
-      </c>
-      <c r="L18" t="s">
-        <v>123</v>
+      <c r="C18" s="1">
+        <v>18364</v>
+      </c>
+      <c r="D18" s="1">
+        <v>16839</v>
+      </c>
+      <c r="E18" s="1">
+        <v>16001</v>
+      </c>
+      <c r="F18" s="1">
+        <v>14571</v>
+      </c>
+      <c r="G18" s="1">
+        <v>14476</v>
+      </c>
+      <c r="H18" s="1">
+        <v>14579</v>
+      </c>
+      <c r="I18" s="1">
+        <v>16569</v>
+      </c>
+      <c r="J18" s="1">
+        <v>18422</v>
+      </c>
+      <c r="K18" s="1">
+        <v>25508</v>
+      </c>
+      <c r="L18" s="1">
+        <v>33953</v>
       </c>
       <c r="M18">
         <v>40767</v>
@@ -2555,11 +3002,11 @@
         <v>39.472204341596459</v>
       </c>
       <c r="Q18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.3508499196618198</v>
       </c>
       <c r="R18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.68891992878085873</v>
       </c>
     </row>
@@ -2570,35 +3017,35 @@
       <c r="B19" t="s">
         <v>128</v>
       </c>
-      <c r="C19" t="s">
-        <v>318</v>
-      </c>
-      <c r="D19" t="s">
-        <v>317</v>
-      </c>
-      <c r="E19" t="s">
-        <v>252</v>
-      </c>
-      <c r="F19" t="s">
-        <v>251</v>
-      </c>
-      <c r="G19" t="s">
-        <v>250</v>
-      </c>
-      <c r="H19" t="s">
-        <v>249</v>
-      </c>
-      <c r="I19" t="s">
-        <v>132</v>
-      </c>
-      <c r="J19" t="s">
-        <v>131</v>
-      </c>
-      <c r="K19" t="s">
-        <v>130</v>
-      </c>
-      <c r="L19" t="s">
-        <v>129</v>
+      <c r="C19" s="1">
+        <v>17182</v>
+      </c>
+      <c r="D19" s="1">
+        <v>17030</v>
+      </c>
+      <c r="E19" s="1">
+        <v>16112</v>
+      </c>
+      <c r="F19" s="1">
+        <v>15189</v>
+      </c>
+      <c r="G19" s="1">
+        <v>14626</v>
+      </c>
+      <c r="H19" s="1">
+        <v>29111</v>
+      </c>
+      <c r="I19" s="1">
+        <v>38915</v>
+      </c>
+      <c r="J19" s="1">
+        <v>47388</v>
+      </c>
+      <c r="K19" s="1">
+        <v>59895</v>
+      </c>
+      <c r="L19" s="1">
+        <v>75974</v>
       </c>
       <c r="M19">
         <v>86520</v>
@@ -2613,11 +3060,11 @@
         <v>38.472476463620808</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.3441274621593273</v>
       </c>
       <c r="R19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.67147138568620757</v>
       </c>
     </row>
@@ -2628,35 +3075,35 @@
       <c r="B20" t="s">
         <v>134</v>
       </c>
-      <c r="C20" t="s">
-        <v>320</v>
-      </c>
-      <c r="D20" t="s">
-        <v>319</v>
-      </c>
-      <c r="E20" t="s">
-        <v>256</v>
-      </c>
-      <c r="F20" t="s">
-        <v>255</v>
-      </c>
-      <c r="G20" t="s">
-        <v>254</v>
-      </c>
-      <c r="H20" t="s">
-        <v>253</v>
-      </c>
-      <c r="I20" t="s">
-        <v>138</v>
-      </c>
-      <c r="J20" t="s">
-        <v>137</v>
-      </c>
-      <c r="K20" t="s">
-        <v>136</v>
-      </c>
-      <c r="L20" t="s">
-        <v>135</v>
+      <c r="C20" s="1">
+        <v>25923</v>
+      </c>
+      <c r="D20" s="1">
+        <v>26455</v>
+      </c>
+      <c r="E20" s="1">
+        <v>24602</v>
+      </c>
+      <c r="F20" s="1">
+        <v>23382</v>
+      </c>
+      <c r="G20" s="1">
+        <v>20965</v>
+      </c>
+      <c r="H20" s="1">
+        <v>20745</v>
+      </c>
+      <c r="I20" s="1">
+        <v>19623</v>
+      </c>
+      <c r="J20" s="1">
+        <v>18924</v>
+      </c>
+      <c r="K20" s="1">
+        <v>19188</v>
+      </c>
+      <c r="L20" s="1">
+        <v>23440</v>
       </c>
       <c r="M20">
         <v>24721</v>
@@ -2671,11 +3118,11 @@
         <v>38.422435231333537</v>
       </c>
       <c r="Q20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.3279000671658934</v>
       </c>
       <c r="R20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.67059800142103942</v>
       </c>
     </row>
@@ -2686,35 +3133,35 @@
       <c r="B21" t="s">
         <v>140</v>
       </c>
-      <c r="C21" t="s">
-        <v>322</v>
-      </c>
-      <c r="D21" t="s">
-        <v>321</v>
-      </c>
-      <c r="E21" t="s">
-        <v>260</v>
-      </c>
-      <c r="F21" t="s">
-        <v>259</v>
-      </c>
-      <c r="G21" t="s">
-        <v>258</v>
-      </c>
-      <c r="H21" t="s">
-        <v>257</v>
-      </c>
-      <c r="I21" t="s">
-        <v>144</v>
-      </c>
-      <c r="J21" t="s">
-        <v>143</v>
-      </c>
-      <c r="K21" t="s">
-        <v>142</v>
-      </c>
-      <c r="L21" t="s">
-        <v>141</v>
+      <c r="C21" s="1">
+        <v>20342</v>
+      </c>
+      <c r="D21" s="1">
+        <v>19620</v>
+      </c>
+      <c r="E21" s="1">
+        <v>18306</v>
+      </c>
+      <c r="F21" s="1">
+        <v>18583</v>
+      </c>
+      <c r="G21" s="1">
+        <v>18784</v>
+      </c>
+      <c r="H21" s="1">
+        <v>19428</v>
+      </c>
+      <c r="I21" s="1">
+        <v>21578</v>
+      </c>
+      <c r="J21" s="1">
+        <v>23682</v>
+      </c>
+      <c r="K21" s="1">
+        <v>25604</v>
+      </c>
+      <c r="L21" s="1">
+        <v>30549</v>
       </c>
       <c r="M21">
         <v>33892</v>
@@ -2729,11 +3176,11 @@
         <v>38.368611970955733</v>
       </c>
       <c r="Q21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.3200425751137295</v>
       </c>
       <c r="R21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.66965860831328849</v>
       </c>
     </row>
@@ -2744,35 +3191,35 @@
       <c r="B22" t="s">
         <v>146</v>
       </c>
-      <c r="C22" t="s">
-        <v>324</v>
-      </c>
-      <c r="D22" t="s">
-        <v>323</v>
-      </c>
-      <c r="E22" t="s">
-        <v>264</v>
-      </c>
-      <c r="F22" t="s">
-        <v>263</v>
-      </c>
-      <c r="G22" t="s">
-        <v>262</v>
-      </c>
-      <c r="H22" t="s">
-        <v>261</v>
-      </c>
-      <c r="I22" t="s">
-        <v>150</v>
-      </c>
-      <c r="J22" t="s">
-        <v>149</v>
-      </c>
-      <c r="K22" t="s">
-        <v>148</v>
-      </c>
-      <c r="L22" t="s">
-        <v>147</v>
+      <c r="C22" s="1">
+        <v>45133</v>
+      </c>
+      <c r="D22" s="1">
+        <v>49617</v>
+      </c>
+      <c r="E22" s="1">
+        <v>59694</v>
+      </c>
+      <c r="F22" s="1">
+        <v>65882</v>
+      </c>
+      <c r="G22" s="1">
+        <v>68838</v>
+      </c>
+      <c r="H22" s="1">
+        <v>78886</v>
+      </c>
+      <c r="I22" s="1">
+        <v>91219</v>
+      </c>
+      <c r="J22" s="1">
+        <v>103829</v>
+      </c>
+      <c r="K22" s="1">
+        <v>113086</v>
+      </c>
+      <c r="L22" s="1">
+        <v>121393</v>
       </c>
       <c r="M22">
         <v>132098</v>
@@ -2787,11 +3234,11 @@
         <v>39.037574072179012</v>
       </c>
       <c r="Q22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.3279113745685873</v>
       </c>
       <c r="R22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.6813341995506943</v>
       </c>
     </row>
@@ -2802,35 +3249,35 @@
       <c r="B23" t="s">
         <v>152</v>
       </c>
-      <c r="C23" t="s">
-        <v>326</v>
-      </c>
-      <c r="D23" t="s">
-        <v>325</v>
-      </c>
-      <c r="E23" t="s">
-        <v>268</v>
-      </c>
-      <c r="F23" t="s">
-        <v>267</v>
-      </c>
-      <c r="G23" t="s">
-        <v>266</v>
-      </c>
-      <c r="H23" t="s">
-        <v>265</v>
-      </c>
-      <c r="I23" t="s">
-        <v>156</v>
-      </c>
-      <c r="J23" t="s">
-        <v>155</v>
-      </c>
-      <c r="K23" t="s">
-        <v>154</v>
-      </c>
-      <c r="L23" t="s">
-        <v>153</v>
+      <c r="C23" s="1">
+        <v>22852</v>
+      </c>
+      <c r="D23" s="1">
+        <v>26815</v>
+      </c>
+      <c r="E23" s="1">
+        <v>28165</v>
+      </c>
+      <c r="F23" s="1">
+        <v>31229</v>
+      </c>
+      <c r="G23" s="1">
+        <v>34530</v>
+      </c>
+      <c r="H23" s="1">
+        <v>39641</v>
+      </c>
+      <c r="I23" s="1">
+        <v>49050</v>
+      </c>
+      <c r="J23" s="1">
+        <v>54236</v>
+      </c>
+      <c r="K23" s="1">
+        <v>64540</v>
+      </c>
+      <c r="L23" s="1">
+        <v>74339</v>
       </c>
       <c r="M23">
         <v>84861</v>
@@ -2845,11 +3292,11 @@
         <v>38.749204394082938</v>
       </c>
       <c r="Q23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.3295447253477237</v>
       </c>
       <c r="R23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.67630119920500165</v>
       </c>
     </row>
@@ -2860,35 +3307,35 @@
       <c r="B24" t="s">
         <v>158</v>
       </c>
-      <c r="C24" t="s">
-        <v>328</v>
-      </c>
-      <c r="D24" t="s">
-        <v>327</v>
-      </c>
-      <c r="E24" t="s">
-        <v>272</v>
-      </c>
-      <c r="F24" t="s">
-        <v>271</v>
-      </c>
-      <c r="G24" t="s">
-        <v>270</v>
-      </c>
-      <c r="H24" t="s">
-        <v>269</v>
-      </c>
-      <c r="I24" t="s">
-        <v>162</v>
-      </c>
-      <c r="J24" t="s">
-        <v>161</v>
-      </c>
-      <c r="K24" t="s">
-        <v>160</v>
-      </c>
-      <c r="L24" t="s">
-        <v>159</v>
+      <c r="C24" s="1">
+        <v>20865</v>
+      </c>
+      <c r="D24" s="1">
+        <v>21841</v>
+      </c>
+      <c r="E24" s="1">
+        <v>22309</v>
+      </c>
+      <c r="F24" s="1">
+        <v>21624</v>
+      </c>
+      <c r="G24" s="1">
+        <v>21245</v>
+      </c>
+      <c r="H24" s="1">
+        <v>23148</v>
+      </c>
+      <c r="I24" s="1">
+        <v>23733</v>
+      </c>
+      <c r="J24" s="1">
+        <v>24442</v>
+      </c>
+      <c r="K24" s="1">
+        <v>30889</v>
+      </c>
+      <c r="L24" s="1">
+        <v>35028</v>
       </c>
       <c r="M24">
         <v>46776</v>
@@ -2903,11 +3350,11 @@
         <v>38.829503399055923</v>
       </c>
       <c r="Q24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.3412347833778639</v>
       </c>
       <c r="R24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.67770268122785549</v>
       </c>
     </row>
@@ -2918,35 +3365,35 @@
       <c r="B25" t="s">
         <v>164</v>
       </c>
-      <c r="C25" t="s">
-        <v>330</v>
-      </c>
-      <c r="D25" t="s">
-        <v>329</v>
-      </c>
-      <c r="E25" t="s">
-        <v>276</v>
-      </c>
-      <c r="F25" t="s">
-        <v>275</v>
-      </c>
-      <c r="G25" t="s">
-        <v>274</v>
-      </c>
-      <c r="H25" t="s">
-        <v>273</v>
-      </c>
-      <c r="I25" t="s">
-        <v>168</v>
-      </c>
-      <c r="J25" t="s">
-        <v>167</v>
-      </c>
-      <c r="K25" t="s">
-        <v>166</v>
-      </c>
-      <c r="L25" t="s">
-        <v>165</v>
+      <c r="C25" s="1">
+        <v>508957</v>
+      </c>
+      <c r="D25" s="1">
+        <v>558485</v>
+      </c>
+      <c r="E25" s="1">
+        <v>733826</v>
+      </c>
+      <c r="F25" s="1">
+        <v>804874</v>
+      </c>
+      <c r="G25" s="1">
+        <v>859100</v>
+      </c>
+      <c r="H25" s="1">
+        <v>949708</v>
+      </c>
+      <c r="I25" s="1">
+        <v>939024</v>
+      </c>
+      <c r="J25" s="1">
+        <v>905759</v>
+      </c>
+      <c r="K25" s="1">
+        <v>786775</v>
+      </c>
+      <c r="L25" s="1">
+        <v>736014</v>
       </c>
       <c r="M25">
         <v>648587</v>
@@ -2961,17 +3408,18 @@
         <v>38.215656003553853</v>
       </c>
       <c r="Q25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.3356622467325878</v>
       </c>
       <c r="R25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.66698902307155261</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>